<commit_message>
-Improving the Layout Design
</commit_message>
<xml_diff>
--- a/Released/BOM/H01R0.xlsx
+++ b/Released/BOM/H01R0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H01R0x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BD1FE6-8690-4B95-9E2F-79C6B1B2733C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C6AE12-BD63-44EC-9188-413D3FBD73D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,16 +304,16 @@
     <t xml:space="preserve"> C3, C5, C6, C8</t>
   </si>
   <si>
-    <t>Conn Unshrouded Header HDR 1 POS Solder ST Top Entry Thru-Hole Carton</t>
-  </si>
-  <si>
-    <t>103327-1</t>
-  </si>
-  <si>
-    <t>https://octopart.com/103327-1-te+connectivity-1934117?r=sp</t>
-  </si>
-  <si>
     <t xml:space="preserve">RGB LED (H01R0) </t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings Unshrouded 1 POS T/H</t>
+  </si>
+  <si>
+    <t>5-146280-1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
   </si>
 </sst>
 </file>
@@ -593,9 +593,6 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -616,6 +613,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -654,7 +654,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2174599</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -995,7 +995,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1056,11 +1056,11 @@
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>2</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1073,11 +1073,11 @@
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <v>44739</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1085,14 +1085,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,21 +1115,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>93</v>
+      <c r="D9" s="38" t="s">
+        <v>94</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F9" s="27">
         <v>1</v>
@@ -1395,7 +1395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="15" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>56</v>
       </c>
@@ -1408,7 +1408,7 @@
       <c r="D23" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="26" t="s">
         <v>58</v>
       </c>
       <c r="F23" s="27">
@@ -1448,7 +1448,7 @@
       <c r="D25" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="26" t="s">
         <v>62</v>
       </c>
       <c r="F25" s="27">
@@ -1478,9 +1478,10 @@
     <hyperlink ref="E10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E9" r:id="rId17" xr:uid="{BB8EBC04-34F6-46CC-B23D-A085867BD835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
-  <drawing r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>